<commit_message>
Analise de requisitos v1
</commit_message>
<xml_diff>
--- a/Planilha MVP 1.xlsx
+++ b/Planilha MVP 1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC3A39-F6B1-420F-9EE9-B836F1C290BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RENDA VAARIAVEL" sheetId="1" r:id="rId1"/>
@@ -13,7 +14,14 @@
     <sheet name="casa" sheetId="5" r:id="rId4"/>
     <sheet name="carro" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -311,7 +319,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
@@ -388,18 +396,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -488,14 +496,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -533,9 +544,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,9 +579,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,9 +631,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -778,7 +823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -800,22 +845,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
       <c r="N2" t="s">
         <v>11</v>
       </c>
@@ -1278,7 +1323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q61"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -1301,24 +1346,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1825,23 +1870,23 @@
       <c r="B39" s="3"/>
     </row>
     <row r="55" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="10" t="s">
+      <c r="I55" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1951,7 +1996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1973,22 +2018,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
       <c r="N2" t="s">
         <v>11</v>
       </c>
@@ -2333,7 +2378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2345,11 +2390,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,25 +2417,25 @@
       <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>46000</v>
       </c>
       <c r="C2">
         <v>46000</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>86400</v>
       </c>
       <c r="C3" t="s">

</xml_diff>

<commit_message>
Definição dos primeiros requisitos
</commit_message>
<xml_diff>
--- a/Planilha MVP 1.xlsx
+++ b/Planilha MVP 1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC3A39-F6B1-420F-9EE9-B836F1C290BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B43BF97-E7A4-4954-AC70-FEFB078BA3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RENDA VAARIAVEL" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="intenções" sheetId="4" r:id="rId3"/>
     <sheet name="casa" sheetId="5" r:id="rId4"/>
     <sheet name="carro" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t>NOME</t>
   </si>
@@ -314,6 +315,39 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>valor carro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor carro </t>
+  </si>
+  <si>
+    <t>valor do carro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anos </t>
+  </si>
+  <si>
+    <t>Taxa de depreciação</t>
+  </si>
+  <si>
+    <t>Valor de depreciação</t>
+  </si>
+  <si>
+    <t>fordk 1.0 TI - vct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carro </t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>preço</t>
+  </si>
+  <si>
+    <t>Desvalorização</t>
   </si>
 </sst>
 </file>
@@ -826,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O23" sqref="O19:O23"/>
     </sheetView>
   </sheetViews>
@@ -2393,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,4 +2745,339 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B64218F-A6D8-4370-BB6B-79A15C661B4D}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1">
+        <v>43000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>359</v>
+      </c>
+      <c r="B2" s="2">
+        <f>A2/B1</f>
+        <v>8.348837209302325E-3</v>
+      </c>
+      <c r="D2">
+        <v>439</v>
+      </c>
+      <c r="E2" s="2">
+        <f>D2/E1</f>
+        <v>6.271428571428571E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>447</v>
+      </c>
+      <c r="B3" s="2">
+        <f>A3/B1</f>
+        <v>1.0395348837209302E-2</v>
+      </c>
+      <c r="D3">
+        <v>600</v>
+      </c>
+      <c r="E3" s="2">
+        <f>D3/E1</f>
+        <v>8.5714285714285719E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>574</v>
+      </c>
+      <c r="B4" s="2">
+        <f>A4/B1</f>
+        <v>1.3348837209302326E-2</v>
+      </c>
+      <c r="D4">
+        <v>800</v>
+      </c>
+      <c r="E4" s="2">
+        <f>D4/E1</f>
+        <v>1.1428571428571429E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>840</v>
+      </c>
+      <c r="B5" s="2">
+        <f>A5/B1</f>
+        <v>1.9534883720930232E-2</v>
+      </c>
+      <c r="D5">
+        <v>1135</v>
+      </c>
+      <c r="E5" s="2">
+        <f>D5/E1</f>
+        <v>1.6214285714285716E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>482</v>
+      </c>
+      <c r="B6" s="2">
+        <f>A6/B1</f>
+        <v>1.1209302325581396E-2</v>
+      </c>
+      <c r="D6">
+        <v>671</v>
+      </c>
+      <c r="E6" s="2">
+        <f>D6/E1</f>
+        <v>9.585714285714286E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>632</v>
+      </c>
+      <c r="B7" s="2">
+        <f>A7/B1</f>
+        <v>1.4697674418604652E-2</v>
+      </c>
+      <c r="D7">
+        <v>955</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7/E1</f>
+        <v>1.3642857142857142E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>482</v>
+      </c>
+      <c r="B8" s="2">
+        <f>A8/B1</f>
+        <v>1.1209302325581396E-2</v>
+      </c>
+      <c r="D8">
+        <v>671</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D8/E1</f>
+        <v>9.585714285714286E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>840</v>
+      </c>
+      <c r="B9" s="2">
+        <f>A9/B1</f>
+        <v>1.9534883720930232E-2</v>
+      </c>
+      <c r="D9">
+        <v>1135</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9/E1</f>
+        <v>1.6214285714285716E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>574</v>
+      </c>
+      <c r="B10" s="2">
+        <f>A10/B1</f>
+        <v>1.3348837209302326E-2</v>
+      </c>
+      <c r="D10">
+        <v>800</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10/E1</f>
+        <v>1.1428571428571429E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>570</v>
+      </c>
+      <c r="B11" s="2">
+        <f>A11/B1</f>
+        <v>1.3255813953488372E-2</v>
+      </c>
+      <c r="D11">
+        <v>840</v>
+      </c>
+      <c r="E11" s="2">
+        <f>D11/E1</f>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13">
+        <v>2019</v>
+      </c>
+      <c r="K13">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14">
+        <v>2018</v>
+      </c>
+      <c r="K14">
+        <v>37852</v>
+      </c>
+      <c r="L14" s="2">
+        <f>1 -K14/K13</f>
+        <v>0.13776765375854216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>43000</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <f>A15*C15</f>
+        <v>8600</v>
+      </c>
+      <c r="J15">
+        <v>2017</v>
+      </c>
+      <c r="K15">
+        <v>35554</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" ref="L15:L17" si="0">1 -K15/K14</f>
+        <v>6.0710134206911182E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A15-D15</f>
+        <v>34400</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D17" si="1">A16*C16</f>
+        <v>3440</v>
+      </c>
+      <c r="J16">
+        <v>2016</v>
+      </c>
+      <c r="K16">
+        <v>34231</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>3.721100298138047E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>A16-D16</f>
+        <v>30960</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>3096</v>
+      </c>
+      <c r="J17">
+        <v>2015</v>
+      </c>
+      <c r="K17">
+        <v>32503</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="0"/>
+        <v>5.048055855803224E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>A15/5</f>
+        <v>8600</v>
+      </c>
+      <c r="B21">
+        <f>A21/5</f>
+        <v>1720</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>